<commit_message>
Listener and Log4j, allure report added
</commit_message>
<xml_diff>
--- a/src/main/java/com/FB/qa/TestData/Book1.xlsx
+++ b/src/main/java/com/FB/qa/TestData/Book1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suraj\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suraj\eclipse-workspace\PageObjModel\src\main\java\com\FB\qa\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FFD81E0-C8BD-4CB7-A3DD-29A6FCC89C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6EB44E-EFC4-454B-99BA-11CEA90097F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{103EFCC0-9D3A-4B05-95F2-548CC27B2B75}"/>
   </bookViews>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -50,7 +48,7 @@
     <t>surajgarud49@gmail.com</t>
   </si>
   <si>
-    <t>Suraj@123</t>
+    <t>************</t>
   </si>
 </sst>
 </file>
@@ -416,7 +414,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,8 +451,8 @@
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{6D0918AA-4C26-4DC4-BB35-9114B6E2E6E2}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{18A51893-11EB-421F-85C6-D2DAFF27F705}"/>
-    <hyperlink ref="B2" r:id="rId3" xr:uid="{4D63B1DD-E5CC-40F5-A484-F11F6C13CA44}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{998FEEC7-9AD4-4C93-9C92-1A1FFF1D476F}"/>
+    <hyperlink ref="B2" r:id="rId3" display="Suraj@123" xr:uid="{4D63B1DD-E5CC-40F5-A484-F11F6C13CA44}"/>
+    <hyperlink ref="B3" r:id="rId4" display="Suraj@123" xr:uid="{998FEEC7-9AD4-4C93-9C92-1A1FFF1D476F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>